<commit_message>
Added a member to Persoonlijk03
</commit_message>
<xml_diff>
--- a/JSON/ClubsNL.xlsx
+++ b/JSON/ClubsNL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petervandenhamer/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petervandenhamer/Developer/Xcode projects/SwiftUI/Photo-Club-Hub/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0835950-2DC9-2C49-911E-756652B3F199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF4F002-B10F-AA45-90D8-314DA6BBCFF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{084E1DFC-5E29-0141-8377-174496560C67}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="51200" windowHeight="26400" xr2:uid="{084E1DFC-5E29-0141-8377-174496560C67}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -282,9 +282,6 @@
     <t>Dick Mandemaker</t>
   </si>
   <si>
-    <t>lege Level2 bestand klaargezet</t>
-  </si>
-  <si>
     <t xml:space="preserve">                        🔵 `museumsAU.level1.json` (Australia)</t>
   </si>
   <si>
@@ -322,6 +319,9 @@
   </si>
   <si>
     <t>(Echte) clubs</t>
+  </si>
+  <si>
+    <t>vrijwel lege Level2 bestand klaargezet</t>
   </si>
 </sst>
 </file>
@@ -1307,7 +1307,7 @@
   <dimension ref="A1:Q49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="141" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1420,7 +1420,7 @@
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1431,7 +1431,7 @@
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1442,7 +1442,7 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1453,7 +1453,7 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1475,7 +1475,7 @@
         <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1486,12 +1486,12 @@
         <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:17">
       <c r="B18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C18">
         <f>SUM(C4:C17)</f>
@@ -1500,7 +1500,7 @@
     </row>
     <row r="19" spans="1:17">
       <c r="B19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C19">
         <f>SUM(C5:C8)-C8</f>
@@ -1512,7 +1512,7 @@
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21" s="44" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D21" s="42"/>
       <c r="E21" s="41" t="s">
@@ -1665,7 +1665,7 @@
         <v>20</v>
       </c>
       <c r="N24" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:17" ht="20" customHeight="1">
@@ -2192,7 +2192,7 @@
     </row>
     <row r="39" spans="1:13" ht="18" thickTop="1" thickBot="1">
       <c r="A39" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C39" s="40">
         <f>1 - C38/D38</f>
@@ -2280,7 +2280,7 @@
         <v>31</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G43" s="32" t="e">
         <f>Table5[[#This Row],[Fotobond]]/(Table5[[#This Row],[Fotobond]]+Table5[[#This Row],[nonFotobond]])</f>
@@ -2379,14 +2379,14 @@
     </row>
     <row r="48" spans="1:13" ht="18" thickTop="1" thickBot="1">
       <c r="A48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C48" s="40">
         <f>1 - C47/D47</f>
         <v>0.2583333333333333</v>
       </c>
       <c r="I48" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="49" ht="17" thickTop="1"/>
@@ -2443,7 +2443,7 @@
       <c r="C4" s="34"/>
       <c r="D4" s="35"/>
     </row>
-    <row r="5" spans="1:4" ht="20">
+    <row r="5" spans="1:4" ht="21">
       <c r="A5" s="39"/>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
@@ -2455,7 +2455,7 @@
       <c r="C6" s="34"/>
       <c r="D6" s="35"/>
     </row>
-    <row r="7" spans="1:4" ht="20">
+    <row r="7" spans="1:4" ht="21">
       <c r="A7" s="39"/>
       <c r="B7" s="34"/>
       <c r="C7" s="34"/>
@@ -2479,7 +2479,7 @@
       <c r="C10" s="34"/>
       <c r="D10" s="35"/>
     </row>
-    <row r="11" spans="1:4" ht="20">
+    <row r="11" spans="1:4" ht="21">
       <c r="A11" s="39"/>
       <c r="B11" s="34"/>
       <c r="C11" s="34"/>
@@ -2503,7 +2503,7 @@
       <c r="C14" s="34"/>
       <c r="D14" s="35"/>
     </row>
-    <row r="15" spans="1:4" ht="20">
+    <row r="15" spans="1:4" ht="21">
       <c r="A15" s="39"/>
       <c r="B15" s="34"/>
       <c r="C15" s="34"/>
@@ -2551,7 +2551,7 @@
       <c r="C22" s="34"/>
       <c r="D22" s="35"/>
     </row>
-    <row r="23" spans="1:4" ht="20">
+    <row r="23" spans="1:4" ht="21">
       <c r="A23" s="39"/>
       <c r="B23" s="34"/>
       <c r="C23" s="34"/>
@@ -2597,7 +2597,7 @@
       <c r="C30" s="34"/>
       <c r="D30" s="34"/>
     </row>
-    <row r="31" spans="1:4" ht="20">
+    <row r="31" spans="1:4" ht="21">
       <c r="A31" s="39"/>
     </row>
     <row r="32" spans="1:4">
@@ -2606,7 +2606,7 @@
     <row r="33" spans="1:1">
       <c r="A33" s="35"/>
     </row>
-    <row r="34" spans="1:1" ht="20">
+    <row r="34" spans="1:1" ht="21">
       <c r="A34" s="39"/>
     </row>
     <row r="35" spans="1:1">

</xml_diff>

<commit_message>
Added support for club fegGemert
</commit_message>
<xml_diff>
--- a/JSON/ClubsNL.xlsx
+++ b/JSON/ClubsNL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petervandenhamer/Developer/Xcode projects/SwiftUI/Photo-Club-Hub/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF4F002-B10F-AA45-90D8-314DA6BBCFF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA668B1D-E879-4F4D-9F94-F951B44FCCDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="600" windowWidth="51200" windowHeight="26400" xr2:uid="{084E1DFC-5E29-0141-8377-174496560C67}"/>
   </bookViews>
@@ -36,8 +36,51 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Peter van den Hamer</author>
+  </authors>
+  <commentList>
+    <comment ref="B35" authorId="0" shapeId="0" xr:uid="{3D59937F-0049-7746-A177-9B1F135C5E2C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Peter van den Hamer:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Werkt met Claude AI</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="96">
   <si>
     <t>Club</t>
   </si>
@@ -63,12 +106,6 @@
     <t>fkGestel</t>
   </si>
   <si>
-    <t>persoonlijk16</t>
-  </si>
-  <si>
-    <t>persoonlijk03</t>
-  </si>
-  <si>
     <t>Peter van den Hamer</t>
   </si>
   <si>
@@ -105,9 +142,6 @@
     <t>❌</t>
   </si>
   <si>
-    <t>leden lijst</t>
-  </si>
-  <si>
     <t>portfolio's</t>
   </si>
   <si>
@@ -171,9 +205,6 @@
     <t>Bram van den Berge</t>
   </si>
   <si>
-    <t>fccSchot71</t>
-  </si>
-  <si>
     <t>fcSchijndel</t>
   </si>
   <si>
@@ -228,9 +259,6 @@
     <t>Peter moet foto's expo van Nov 2025 nog toevoegen.</t>
   </si>
   <si>
-    <t>moet nog starten met Level 2 bestand.</t>
-  </si>
-  <si>
     <t>clubs in afdeling</t>
   </si>
   <si>
@@ -322,6 +350,24 @@
   </si>
   <si>
     <t>vrijwel lege Level2 bestand klaargezet</t>
+  </si>
+  <si>
+    <t>Peter van Gils</t>
+  </si>
+  <si>
+    <t>fegGemert</t>
+  </si>
+  <si>
+    <t>ffcShot71</t>
+  </si>
+  <si>
+    <t>leden lijst &amp; link</t>
+  </si>
+  <si>
+    <t>Persoonlijk16</t>
+  </si>
+  <si>
+    <t>Persoonlijk03</t>
   </si>
 </sst>
 </file>
@@ -331,7 +377,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -400,6 +446,19 @@
       <sz val="16"/>
       <color rgb="FF666666"/>
       <name val="Inherit"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -563,7 +622,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -675,6 +734,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -686,6 +763,26 @@
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="24">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -708,12 +805,6 @@
     </dxf>
     <dxf>
       <alignment vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -757,20 +848,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -926,10 +1003,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7BFB9A37-6C77-C04D-823C-1F22CEC41A47}" name="Table1" displayName="Table1" ref="A22:N37" totalsRowShown="0" headerRowDxfId="23" headerRowCellStyle="Comma">
-  <autoFilter ref="A22:N37" xr:uid="{7BFB9A37-6C77-C04D-823C-1F22CEC41A47}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A23:N37">
-    <sortCondition descending="1" ref="D22:D37"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7BFB9A37-6C77-C04D-823C-1F22CEC41A47}" name="Table1" displayName="Table1" ref="A22:N38" totalsRowShown="0" headerRowDxfId="23" headerRowCellStyle="Comma">
+  <autoFilter ref="A22:N38" xr:uid="{7BFB9A37-6C77-C04D-823C-1F22CEC41A47}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A23:N38">
+    <sortCondition descending="1" ref="D22:D38"/>
   </sortState>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{16FD4912-2777-D44B-BAA2-DF72031A6FBF}" name="Club" dataDxfId="22"/>
@@ -938,42 +1015,42 @@
     <tableColumn id="4" xr3:uid="{5743EC05-499D-2A43-B382-184D22CD50BC}" name="volgens website" dataDxfId="19"/>
     <tableColumn id="5" xr3:uid="{2A142040-356D-8A4F-8279-E185EB2BC50B}" name="club op kaart" dataDxfId="18"/>
     <tableColumn id="6" xr3:uid="{3CC810E5-003B-F74C-9504-4ED2036DE1E7}" name="club website" dataDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{C1634577-561E-5D4B-BB23-133C51958BDB}" name="leden lijst" dataDxfId="16"/>
-    <tableColumn id="8" xr3:uid="{2C9F80B9-0340-5A4D-BC64-757304D12D92}" name="featured image" dataDxfId="15"/>
-    <tableColumn id="9" xr3:uid="{C5C64B85-895C-C244-9352-A9F04BB3AD08}" name="expertises" dataDxfId="14"/>
-    <tableColumn id="10" xr3:uid="{FAC779F1-11AB-8D4D-89DB-0C843273A450}" name="lid website" dataDxfId="13"/>
-    <tableColumn id="11" xr3:uid="{ECF8E65C-7B1A-CE46-A0C7-46174388719C}" name="bestuursleden" dataDxfId="12"/>
-    <tableColumn id="12" xr3:uid="{20592BBE-01DC-8F47-9DB6-133915F7B829}" name="portfolio's" dataDxfId="11"/>
-    <tableColumn id="13" xr3:uid="{509BD853-42B7-7448-B3DA-B0AD4A518221}" name="Momenteel actief" dataDxfId="10"/>
-    <tableColumn id="14" xr3:uid="{CB3FDBB9-8552-6044-989A-BF48D73BB53D}" name="Opmerking" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{C1634577-561E-5D4B-BB23-133C51958BDB}" name="leden lijst &amp; link" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{2C9F80B9-0340-5A4D-BC64-757304D12D92}" name="featured image" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{C5C64B85-895C-C244-9352-A9F04BB3AD08}" name="expertises" dataDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{FAC779F1-11AB-8D4D-89DB-0C843273A450}" name="lid website" dataDxfId="15"/>
+    <tableColumn id="11" xr3:uid="{ECF8E65C-7B1A-CE46-A0C7-46174388719C}" name="bestuursleden" dataDxfId="14"/>
+    <tableColumn id="12" xr3:uid="{20592BBE-01DC-8F47-9DB6-133915F7B829}" name="portfolio's" dataDxfId="13"/>
+    <tableColumn id="13" xr3:uid="{509BD853-42B7-7448-B3DA-B0AD4A518221}" name="Momenteel actief" dataDxfId="12"/>
+    <tableColumn id="14" xr3:uid="{CB3FDBB9-8552-6044-989A-BF48D73BB53D}" name="Opmerking" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{64122FD9-0012-974E-8524-BD3E0FFEF173}" name="Table5" displayName="Table5" ref="A41:I45" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="A41:I45" xr:uid="{64122FD9-0012-974E-8524-BD3E0FFEF173}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A42:I45">
-    <sortCondition descending="1" ref="E41:E45"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{64122FD9-0012-974E-8524-BD3E0FFEF173}" name="Table5" displayName="Table5" ref="A42:I46" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A42:I46" xr:uid="{64122FD9-0012-974E-8524-BD3E0FFEF173}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A43:I46">
+    <sortCondition descending="1" ref="E42:E46"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{5C79ADE5-E9D4-764E-A62E-ED1B23E337E8}" name="Afdeling"/>
     <tableColumn id="2" xr3:uid="{ED07554A-6159-5543-B1DA-61CB0A7B6C0A}" name="contact voor app"/>
-    <tableColumn id="3" xr3:uid="{92527A9E-5DF3-364B-8235-7C4E537AA579}" name="clubs in app" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{07E2AC0A-3AAB-F444-902C-A129018B5327}" name="clubs in afdeling" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{87F1F381-FA3E-8D40-851D-A4F7993752DE}" name="Fotobond" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{A9CF5635-EBAD-B040-BF71-3E77E09BBB43}" name="nonFotobond" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{5C084667-3F83-6F4E-8687-1A7FBBF558C2}" name="% Fotobond" dataDxfId="3" dataCellStyle="Percent"/>
-    <tableColumn id="7" xr3:uid="{24532655-7031-274B-854D-128E98E3B718}" name="Moment actief" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{A8142398-B094-F849-B96E-739B6E42C1DA}" name="Opmerking" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{92527A9E-5DF3-364B-8235-7C4E537AA579}" name="clubs in app" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{07E2AC0A-3AAB-F444-902C-A129018B5327}" name="clubs in afdeling" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{87F1F381-FA3E-8D40-851D-A4F7993752DE}" name="Fotobond" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{A9CF5635-EBAD-B040-BF71-3E77E09BBB43}" name="nonFotobond" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{5C084667-3F83-6F4E-8687-1A7FBBF558C2}" name="% Fotobond" dataDxfId="0" dataCellStyle="Percent"/>
+    <tableColumn id="7" xr3:uid="{24532655-7031-274B-854D-128E98E3B718}" name="Moment actief" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{A8142398-B094-F849-B96E-739B6E42C1DA}" name="Opmerking" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0EC1E894-FF62-D94F-86C9-0F118170FA74}" name="Table2" displayName="Table2" ref="B3:D17" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0EC1E894-FF62-D94F-86C9-0F118170FA74}" name="Table2" displayName="Table2" ref="B3:D17" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="B3:D17" xr:uid="{0EC1E894-FF62-D94F-86C9-0F118170FA74}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8B16138C-6720-474D-87C6-17E647EE5905}" name="beheerder"/>
@@ -1300,14 +1377,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7C40026-93EC-6A48-ADED-7C2F14F32A0C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7C40026-93EC-6A48-ADED-7C2F14F32A0C}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q49"/>
+  <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="141" workbookViewId="0">
-      <selection activeCell="N39" sqref="N39"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="141" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1318,7 +1395,8 @@
     <col min="4" max="4" width="18.5" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" customWidth="1"/>
     <col min="6" max="6" width="12.1640625" customWidth="1"/>
-    <col min="7" max="8" width="14" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
     <col min="9" max="10" width="12.33203125" customWidth="1"/>
     <col min="11" max="11" width="13.33203125" customWidth="1"/>
     <col min="12" max="12" width="12.33203125" customWidth="1"/>
@@ -1330,168 +1408,170 @@
     <col min="10000" max="16384" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:7" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="36" customFormat="1">
+        <v>42</v>
+      </c>
+      <c r="G1" s="7"/>
+    </row>
+    <row r="3" spans="1:7" s="36" customFormat="1">
       <c r="B3" s="37" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>73</v>
+      </c>
+      <c r="G3" s="46"/>
+    </row>
+    <row r="4" spans="1:7">
       <c r="B4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="B5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="B6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C6">
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="B7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C7">
         <v>79</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="B8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="B9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C9">
         <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="B10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10">
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="B11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C11">
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="B12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="B13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C13">
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="B14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="B15" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C15">
         <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="B16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C16">
         <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:17">
       <c r="B18" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C18">
         <f>SUM(C4:C17)</f>
@@ -1500,7 +1580,7 @@
     </row>
     <row r="19" spans="1:17">
       <c r="B19" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C19">
         <f>SUM(C5:C8)-C8</f>
@@ -1512,22 +1592,22 @@
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21" s="44" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D21" s="42"/>
       <c r="E21" s="41" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F21" s="42"/>
       <c r="G21" s="41" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H21" s="43"/>
       <c r="I21" s="43"/>
       <c r="J21" s="43"/>
       <c r="K21" s="42"/>
       <c r="L21" s="38" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="M21"/>
       <c r="N21"/>
@@ -1540,43 +1620,43 @@
         <v>0</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>22</v>
+        <v>93</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I22" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="J22" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="K22" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="L22" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="M22" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="N22" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="J22" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="K22" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="L22" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="M22" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="N22" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="O22"/>
       <c r="P22"/>
@@ -1584,10 +1664,10 @@
     </row>
     <row r="23" spans="1:17" ht="20" customHeight="1">
       <c r="A23" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C23" s="22">
         <v>0</v>
@@ -1596,40 +1676,40 @@
         <v>35</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F23" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>21</v>
+        <v>18</v>
+      </c>
+      <c r="G23" s="45" t="s">
+        <v>19</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J23" s="26" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K23" s="25" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L23" s="27" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M23" s="5"/>
       <c r="N23" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:17" ht="20" customHeight="1">
       <c r="A24" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B24" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C24" s="24">
         <v>1</v>
@@ -1638,34 +1718,34 @@
         <v>35</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G24" s="12" t="s">
-        <v>21</v>
+        <v>18</v>
+      </c>
+      <c r="G24" s="47" t="s">
+        <v>25</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J24" s="26" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K24" s="25" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L24" s="27" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M24" s="26" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="N24" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:17" ht="20" customHeight="1">
@@ -1673,7 +1753,7 @@
         <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C25" s="24">
         <v>23</v>
@@ -1682,28 +1762,28 @@
         <v>22</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F25" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="G25" s="45" t="s">
+        <v>18</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J25" s="3">
         <v>7</v>
       </c>
       <c r="K25" s="25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L25" s="28" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="M25" s="3"/>
     </row>
@@ -1712,7 +1792,7 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C26" s="21">
         <v>22</v>
@@ -1721,34 +1801,34 @@
         <v>22</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G26" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="G26" s="45" t="s">
+        <v>18</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J26" s="3">
         <v>8</v>
       </c>
       <c r="K26" s="13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L26" s="28" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="N26" s="30" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="20" customHeight="1">
@@ -1756,7 +1836,7 @@
         <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C27" s="24">
         <v>18</v>
@@ -1765,28 +1845,28 @@
         <v>19</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="G27" s="45" t="s">
+        <v>18</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J27" s="29">
         <v>1</v>
       </c>
       <c r="K27" s="25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L27" s="28" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="M27" s="3"/>
     </row>
@@ -1795,7 +1875,7 @@
         <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C28" s="24">
         <v>19</v>
@@ -1804,28 +1884,28 @@
         <v>18</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G28" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="G28" s="45" t="s">
+        <v>18</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J28" s="29">
         <v>3</v>
       </c>
       <c r="K28" s="25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L28" s="28" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="M28" s="3"/>
     </row>
@@ -1834,7 +1914,7 @@
         <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C29" s="24">
         <v>19</v>
@@ -1843,28 +1923,28 @@
         <v>18</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F29" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="G29" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="G29" s="45" t="s">
+        <v>18</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J29" s="29">
         <v>3</v>
       </c>
       <c r="K29" s="13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L29" s="28" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="M29" s="3"/>
     </row>
@@ -1873,7 +1953,7 @@
         <v>7</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C30" s="24">
         <v>11</v>
@@ -1882,76 +1962,76 @@
         <v>17</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G30" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G30" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="H30" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H30" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="I30" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J30" s="29">
         <v>0</v>
       </c>
       <c r="K30" s="25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L30" s="28" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="M30" s="26" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="N30" s="30" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:17" ht="20" customHeight="1">
-      <c r="A31" t="s">
-        <v>44</v>
-      </c>
-      <c r="B31" t="s">
-        <v>18</v>
-      </c>
-      <c r="C31" s="24">
+      <c r="A31" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="B31" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="48">
         <v>1</v>
       </c>
-      <c r="D31" s="13">
+      <c r="D31" s="49">
         <v>16</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F31" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="G31" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I31" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J31" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="K31" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="L31" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="M31" s="3"/>
-      <c r="N31" t="s">
-        <v>63</v>
+        <v>18</v>
+      </c>
+      <c r="F31" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="H31" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="I31" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="J31" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="K31" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="L31" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="M31" s="47"/>
+      <c r="N31" s="35" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:17" ht="20" customHeight="1">
@@ -1959,7 +2039,7 @@
         <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C32" s="21">
         <v>11</v>
@@ -1968,37 +2048,37 @@
         <v>11</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F32" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G32" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="G32" s="45" t="s">
+        <v>18</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J32" s="29">
         <v>0</v>
       </c>
       <c r="K32" s="25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L32" s="28" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M32" s="3"/>
     </row>
-    <row r="33" spans="1:13" ht="20" customHeight="1">
+    <row r="33" spans="1:14" ht="20" customHeight="1">
       <c r="A33" t="s">
-        <v>8</v>
+        <v>94</v>
       </c>
       <c r="B33" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C33" s="21">
         <v>10</v>
@@ -2007,404 +2087,463 @@
         <v>10</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F33" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="G33" s="12" t="s">
-        <v>20</v>
+        <v>55</v>
+      </c>
+      <c r="G33" s="45" t="s">
+        <v>18</v>
       </c>
       <c r="H33" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I33" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="I33" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="J33" s="3">
         <v>6</v>
       </c>
       <c r="K33" s="13" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="L33" s="28" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="M33" s="26" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" ht="20" customHeight="1">
-      <c r="A34" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C34" s="22">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="20" customHeight="1">
+      <c r="A34" t="s">
+        <v>95</v>
+      </c>
+      <c r="B34" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="24">
+        <v>1</v>
+      </c>
+      <c r="D34" s="13">
+        <v>1</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F34" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="G34" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J34" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="K34" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="L34" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="M34" s="3"/>
+    </row>
+    <row r="35" spans="1:14" ht="20" customHeight="1">
+      <c r="A35" t="s">
+        <v>91</v>
+      </c>
+      <c r="B35" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35" s="24">
+        <v>1</v>
+      </c>
+      <c r="D35" s="13">
+        <v>14</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G35" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J35" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="K35" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="L35" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="M35" s="3"/>
+      <c r="N35" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="20" customHeight="1">
+      <c r="A36" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="22">
         <v>2</v>
       </c>
-      <c r="D34" s="23">
+      <c r="D36" s="23">
         <v>2</v>
       </c>
-      <c r="E34" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F34" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="G34" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I34" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="J34" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="K34" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="L34" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="M34" s="26" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" ht="20" customHeight="1">
-      <c r="A35" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C35" s="22">
+      <c r="E36" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="G36" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K36" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="L36" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="M36" s="26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="20" customHeight="1">
+      <c r="A37" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="22">
         <v>2</v>
       </c>
-      <c r="D35" s="23">
+      <c r="D37" s="23">
         <v>2</v>
       </c>
-      <c r="E35" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F35" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G35" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J35" s="3">
+      <c r="E37" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F37" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G37" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J37" s="3">
         <v>1</v>
       </c>
-      <c r="K35" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="L35" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="M35" s="26" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" ht="20" customHeight="1">
-      <c r="A36" t="s">
-        <v>9</v>
-      </c>
-      <c r="B36" t="s">
-        <v>17</v>
-      </c>
-      <c r="C36" s="24">
-        <v>0</v>
-      </c>
-      <c r="D36" s="13">
-        <v>1</v>
-      </c>
-      <c r="E36" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F36" s="23" t="s">
+      <c r="K37" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="L37" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="M37" s="26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="20" customHeight="1" thickBot="1">
+      <c r="C38" s="21"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="13"/>
+      <c r="L38" s="28"/>
+      <c r="M38" s="3"/>
+    </row>
+    <row r="39" spans="1:14" ht="18" thickTop="1" thickBot="1">
+      <c r="A39" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" s="9">
+        <f>SUM(C23:C37)</f>
+        <v>141</v>
+      </c>
+      <c r="D39" s="9">
+        <f>SUM(D23:D37)</f>
+        <v>242</v>
+      </c>
+      <c r="E39" s="14"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="12"/>
+      <c r="J39" s="9">
+        <f>SUM(J23:J37)</f>
+        <v>29</v>
+      </c>
+      <c r="K39" s="15"/>
+      <c r="L39" s="19"/>
+    </row>
+    <row r="40" spans="1:14" ht="18" thickTop="1" thickBot="1">
+      <c r="A40" t="s">
+        <v>83</v>
+      </c>
+      <c r="C40" s="40">
+        <f>1 - C39/D39</f>
+        <v>0.4173553719008265</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="17" thickTop="1">
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="A42" t="s">
+        <v>60</v>
+      </c>
+      <c r="B42" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D42" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="G36" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J36" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="K36" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="L36" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="M36" s="3"/>
-    </row>
-    <row r="37" spans="1:13" ht="20" customHeight="1" thickBot="1">
-      <c r="C37" s="21"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="12"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="13"/>
-      <c r="L37" s="28"/>
-      <c r="M37" s="3"/>
-    </row>
-    <row r="38" spans="1:13" ht="18" thickTop="1" thickBot="1">
-      <c r="A38" t="s">
-        <v>42</v>
-      </c>
-      <c r="C38" s="9">
-        <f>SUM(C23:C33,C36)</f>
-        <v>135</v>
-      </c>
-      <c r="D38" s="9">
-        <f>SUM(D23:D33,D36)</f>
-        <v>224</v>
-      </c>
-      <c r="E38" s="14"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="14"/>
-      <c r="J38" s="9">
-        <f>SUM(J23:J33,J36)</f>
-        <v>28</v>
-      </c>
-      <c r="K38" s="15"/>
-      <c r="L38" s="19"/>
-    </row>
-    <row r="39" spans="1:13" ht="18" thickTop="1" thickBot="1">
-      <c r="A39" t="s">
-        <v>88</v>
-      </c>
-      <c r="C39" s="40">
-        <f>1 - C38/D38</f>
-        <v>0.3973214285714286</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" ht="17" thickTop="1">
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-    </row>
-    <row r="41" spans="1:13">
-      <c r="A41" t="s">
+      <c r="E42" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B41" t="s">
-        <v>67</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D41" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H41" s="2" t="s">
+      <c r="F42" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="I41" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" ht="20" customHeight="1">
-      <c r="A42" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C42" s="5">
+      <c r="G42" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" ht="20" customHeight="1">
+      <c r="A43" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="5">
         <v>2</v>
       </c>
-      <c r="D42" s="5">
+      <c r="D43" s="5">
         <f>SUM(Table5[[#This Row],[Fotobond]:[nonFotobond]])</f>
         <v>2</v>
       </c>
-      <c r="E42" s="5">
+      <c r="E43" s="5">
         <v>0</v>
       </c>
-      <c r="F42" s="5">
+      <c r="F43" s="5">
         <v>2</v>
       </c>
-      <c r="G42" s="33" t="s">
-        <v>72</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I42" s="3"/>
-    </row>
-    <row r="43" spans="1:13" ht="20" customHeight="1">
-      <c r="A43" t="s">
-        <v>25</v>
-      </c>
-      <c r="B43" t="s">
-        <v>29</v>
-      </c>
-      <c r="C43" s="5">
+      <c r="G43" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I43" s="3"/>
+    </row>
+    <row r="44" spans="1:14" ht="20" customHeight="1">
+      <c r="A44" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44" t="s">
+        <v>26</v>
+      </c>
+      <c r="C44" s="5">
         <v>0</v>
       </c>
-      <c r="D43" s="3">
+      <c r="D44" s="3">
         <f>SUM(Table5[[#This Row],[Fotobond]:[nonFotobond]])</f>
         <v>31</v>
       </c>
-      <c r="E43" s="3">
+      <c r="E44" s="3">
         <v>31</v>
       </c>
-      <c r="F43" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G43" s="32" t="e">
+      <c r="F44" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G44" s="32" t="e">
         <f>Table5[[#This Row],[Fotobond]]/(Table5[[#This Row],[Fotobond]]+Table5[[#This Row],[nonFotobond]])</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="20" customHeight="1">
-      <c r="A44" t="s">
-        <v>24</v>
-      </c>
-      <c r="B44" t="s">
-        <v>61</v>
-      </c>
-      <c r="C44" s="3">
+    <row r="45" spans="1:14" ht="20" customHeight="1">
+      <c r="A45" t="s">
+        <v>21</v>
+      </c>
+      <c r="B45" t="s">
+        <v>57</v>
+      </c>
+      <c r="C45" s="3">
         <v>79</v>
       </c>
-      <c r="D44" s="3">
+      <c r="D45" s="3">
         <f>SUM(Table5[[#This Row],[Fotobond]:[nonFotobond]])</f>
         <v>79</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E45" s="3">
         <v>29</v>
       </c>
-      <c r="F44" s="3">
+      <c r="F45" s="3">
         <v>50</v>
       </c>
-      <c r="G44" s="32">
+      <c r="G45" s="32">
         <f>Table5[[#This Row],[Fotobond]]/(Table5[[#This Row],[Fotobond]]+Table5[[#This Row],[nonFotobond]])</f>
         <v>0.36708860759493672</v>
       </c>
-      <c r="H44" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I44" s="3"/>
-    </row>
-    <row r="45" spans="1:13" ht="20" customHeight="1">
-      <c r="A45" t="s">
-        <v>26</v>
-      </c>
-      <c r="B45" t="s">
-        <v>17</v>
-      </c>
-      <c r="C45" s="3">
+      <c r="H45" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I45" s="3"/>
+    </row>
+    <row r="46" spans="1:14" ht="20" customHeight="1">
+      <c r="A46" t="s">
+        <v>23</v>
+      </c>
+      <c r="B46" t="s">
+        <v>15</v>
+      </c>
+      <c r="C46" s="3">
         <v>10</v>
       </c>
-      <c r="D45" s="3">
+      <c r="D46" s="3">
         <f>Table5[[#This Row],[Fotobond]]+Table5[[#This Row],[nonFotobond]]</f>
         <v>10</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E46" s="3">
         <v>6</v>
       </c>
-      <c r="F45" s="3">
+      <c r="F46" s="3">
         <v>4</v>
       </c>
-      <c r="G45" s="32">
+      <c r="G46" s="32">
         <f>Table5[[#This Row],[Fotobond]]/(Table5[[#This Row],[Fotobond]]+Table5[[#This Row],[nonFotobond]])</f>
         <v>0.6</v>
       </c>
-      <c r="H45" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I45" s="31" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" ht="17" thickBot="1">
-      <c r="A46" s="4"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="3"/>
-    </row>
-    <row r="47" spans="1:13" ht="18" thickTop="1" thickBot="1">
-      <c r="A47" t="s">
-        <v>42</v>
-      </c>
-      <c r="C47" s="9">
-        <f>SUM(C43:C45)</f>
+      <c r="H46" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I46" s="31" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="17" thickBot="1">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+    </row>
+    <row r="48" spans="1:14" ht="18" thickTop="1" thickBot="1">
+      <c r="A48" t="s">
+        <v>39</v>
+      </c>
+      <c r="C48" s="9">
+        <f>SUM(C44:C46)</f>
         <v>89</v>
       </c>
-      <c r="D47" s="9">
-        <f>SUM(D43:D45)</f>
+      <c r="D48" s="9">
+        <f>SUM(D44:D46)</f>
         <v>120</v>
       </c>
-      <c r="E47" s="9">
-        <f>SUM(E43:E45)</f>
+      <c r="E48" s="9">
+        <f>SUM(E44:E46)</f>
         <v>66</v>
       </c>
-      <c r="F47" s="9">
-        <f>SUM(F43:F45)</f>
+      <c r="F48" s="9">
+        <f>SUM(F44:F46)</f>
         <v>54</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="18" thickTop="1" thickBot="1">
-      <c r="A48" t="s">
-        <v>89</v>
-      </c>
-      <c r="C48" s="40">
-        <f>1 - C47/D47</f>
+    <row r="49" spans="1:9" ht="18" thickTop="1" thickBot="1">
+      <c r="A49" t="s">
+        <v>84</v>
+      </c>
+      <c r="C49" s="40">
+        <f>1 - C48/D48</f>
         <v>0.2583333333333333</v>
       </c>
-      <c r="I48" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="49" ht="17" thickTop="1"/>
+      <c r="I49" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="17" thickTop="1"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="G21:K21"/>
     <mergeCell ref="C21:D21"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G24" r:id="rId1" xr:uid="{6B877BCA-FAC0-CA45-A9F8-5DB8E2862E74}"/>
+    <hyperlink ref="G30" r:id="rId2" xr:uid="{EA518462-58C1-0D43-AFAB-D0D435BCFCF8}"/>
+    <hyperlink ref="G31" r:id="rId3" xr:uid="{D509616D-ADA9-DE4E-85FF-FE0FAAE01599}"/>
+    <hyperlink ref="G34" r:id="rId4" xr:uid="{C029A8E2-CAAD-E34C-A625-21082F80D214}"/>
+    <hyperlink ref="G25" r:id="rId5" xr:uid="{300B6D68-2854-B547-8455-4CF19B28FACA}"/>
+    <hyperlink ref="G26" r:id="rId6" xr:uid="{64CE12B8-0756-494D-9F75-5BA28534233A}"/>
+    <hyperlink ref="G27" r:id="rId7" xr:uid="{4FAAD59B-10D8-B041-B48F-94650351060E}"/>
+    <hyperlink ref="G28" r:id="rId8" xr:uid="{3D6FECDE-2356-C54B-AD91-964D700B8CA2}"/>
+    <hyperlink ref="G29" r:id="rId9" xr:uid="{16FF2E58-7A12-6C40-B212-0FFEAE348999}"/>
+    <hyperlink ref="G32" r:id="rId10" xr:uid="{2844051E-41E4-F049-B6A5-3C772738F0F7}"/>
+    <hyperlink ref="G33" r:id="rId11" xr:uid="{95C73904-B606-134B-98EE-809F1208E9C4}"/>
+    <hyperlink ref="G35" r:id="rId12" xr:uid="{D27CFD2E-6D1C-B942-87DB-7A59EDCEE61A}"/>
+    <hyperlink ref="G36" r:id="rId13" xr:uid="{4BFA2C99-59DE-554B-B537-03CA48FE83E5}"/>
+    <hyperlink ref="G37" r:id="rId14" xr:uid="{AB835A00-2A8B-8C40-9BEE-3D0305CB9D21}"/>
+    <hyperlink ref="G23" r:id="rId15" xr:uid="{A9A1726F-23F6-EA4D-A625-108B0892EFF4}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="53" orientation="landscape" horizontalDpi="0" verticalDpi="0" copies="6"/>
   <ignoredErrors>
-    <ignoredError sqref="C47" formulaRange="1"/>
+    <ignoredError sqref="C48" formulaRange="1"/>
   </ignoredErrors>
+  <legacyDrawing r:id="rId16"/>
   <tableParts count="3">
-    <tablePart r:id="rId1"/>
-    <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId17"/>
+    <tablePart r:id="rId18"/>
+    <tablePart r:id="rId19"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Step in fixing merge conflict issues. Main branch will temporarily give a few compiler errors.
</commit_message>
<xml_diff>
--- a/JSON/ClubsNL.xlsx
+++ b/JSON/ClubsNL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10201"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petervandenhamer/Developer/Xcode projects/SwiftUI/Photo-Club-Hub/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA668B1D-E879-4F4D-9F94-F951B44FCCDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D4D29F-0605-7D4A-AA86-ABDDC84BBADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="600" windowWidth="51200" windowHeight="26400" xr2:uid="{084E1DFC-5E29-0141-8377-174496560C67}"/>
   </bookViews>
@@ -42,6 +42,39 @@
     <author>Peter van den Hamer</author>
   </authors>
   <commentList>
+    <comment ref="B24" authorId="0" shapeId="0" xr:uid="{EE24AEB8-A4ED-AD48-85DE-42F41285BA7D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Peter van den Hamer:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>en Dick Mandemaker</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B35" authorId="0" shapeId="0" xr:uid="{3D59937F-0049-7746-A177-9B1F135C5E2C}">
       <text>
         <r>
@@ -80,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="97">
   <si>
     <t>Club</t>
   </si>
@@ -307,9 +340,6 @@
     <t>fcVeghel</t>
   </si>
   <si>
-    <t>Dick Mandemaker</t>
-  </si>
-  <si>
     <t xml:space="preserve">                        🔵 `museumsAU.level1.json` (Australia)</t>
   </si>
   <si>
@@ -368,6 +398,12 @@
   </si>
   <si>
     <t>Persoonlijk03</t>
+  </si>
+  <si>
+    <t>Harry Michiels</t>
+  </si>
+  <si>
+    <t>besproken/goedgekeurd in ALV op 5Feb26</t>
   </si>
 </sst>
 </file>
@@ -724,6 +760,24 @@
     <xf numFmtId="9" fontId="2" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -734,24 +788,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -763,26 +799,6 @@
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="24">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -805,6 +821,12 @@
     </dxf>
     <dxf>
       <alignment vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -848,6 +870,20 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1015,21 +1051,21 @@
     <tableColumn id="4" xr3:uid="{5743EC05-499D-2A43-B382-184D22CD50BC}" name="volgens website" dataDxfId="19"/>
     <tableColumn id="5" xr3:uid="{2A142040-356D-8A4F-8279-E185EB2BC50B}" name="club op kaart" dataDxfId="18"/>
     <tableColumn id="6" xr3:uid="{3CC810E5-003B-F74C-9504-4ED2036DE1E7}" name="club website" dataDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{C1634577-561E-5D4B-BB23-133C51958BDB}" name="leden lijst &amp; link" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{2C9F80B9-0340-5A4D-BC64-757304D12D92}" name="featured image" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{C5C64B85-895C-C244-9352-A9F04BB3AD08}" name="expertises" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{FAC779F1-11AB-8D4D-89DB-0C843273A450}" name="lid website" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{ECF8E65C-7B1A-CE46-A0C7-46174388719C}" name="bestuursleden" dataDxfId="14"/>
-    <tableColumn id="12" xr3:uid="{20592BBE-01DC-8F47-9DB6-133915F7B829}" name="portfolio's" dataDxfId="13"/>
-    <tableColumn id="13" xr3:uid="{509BD853-42B7-7448-B3DA-B0AD4A518221}" name="Momenteel actief" dataDxfId="12"/>
-    <tableColumn id="14" xr3:uid="{CB3FDBB9-8552-6044-989A-BF48D73BB53D}" name="Opmerking" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{C1634577-561E-5D4B-BB23-133C51958BDB}" name="leden lijst &amp; link" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{2C9F80B9-0340-5A4D-BC64-757304D12D92}" name="featured image" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{C5C64B85-895C-C244-9352-A9F04BB3AD08}" name="expertises" dataDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{FAC779F1-11AB-8D4D-89DB-0C843273A450}" name="lid website" dataDxfId="13"/>
+    <tableColumn id="11" xr3:uid="{ECF8E65C-7B1A-CE46-A0C7-46174388719C}" name="bestuursleden" dataDxfId="12"/>
+    <tableColumn id="12" xr3:uid="{20592BBE-01DC-8F47-9DB6-133915F7B829}" name="portfolio's" dataDxfId="11"/>
+    <tableColumn id="13" xr3:uid="{509BD853-42B7-7448-B3DA-B0AD4A518221}" name="Momenteel actief" dataDxfId="10"/>
+    <tableColumn id="14" xr3:uid="{CB3FDBB9-8552-6044-989A-BF48D73BB53D}" name="Opmerking" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{64122FD9-0012-974E-8524-BD3E0FFEF173}" name="Table5" displayName="Table5" ref="A42:I46" totalsRowShown="0" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{64122FD9-0012-974E-8524-BD3E0FFEF173}" name="Table5" displayName="Table5" ref="A42:I46" totalsRowShown="0" headerRowDxfId="8">
   <autoFilter ref="A42:I46" xr:uid="{64122FD9-0012-974E-8524-BD3E0FFEF173}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A43:I46">
     <sortCondition descending="1" ref="E42:E46"/>
@@ -1037,20 +1073,20 @@
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{5C79ADE5-E9D4-764E-A62E-ED1B23E337E8}" name="Afdeling"/>
     <tableColumn id="2" xr3:uid="{ED07554A-6159-5543-B1DA-61CB0A7B6C0A}" name="contact voor app"/>
-    <tableColumn id="3" xr3:uid="{92527A9E-5DF3-364B-8235-7C4E537AA579}" name="clubs in app" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{07E2AC0A-3AAB-F444-902C-A129018B5327}" name="clubs in afdeling" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{87F1F381-FA3E-8D40-851D-A4F7993752DE}" name="Fotobond" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{A9CF5635-EBAD-B040-BF71-3E77E09BBB43}" name="nonFotobond" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{5C084667-3F83-6F4E-8687-1A7FBBF558C2}" name="% Fotobond" dataDxfId="0" dataCellStyle="Percent"/>
-    <tableColumn id="7" xr3:uid="{24532655-7031-274B-854D-128E98E3B718}" name="Moment actief" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{A8142398-B094-F849-B96E-739B6E42C1DA}" name="Opmerking" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{92527A9E-5DF3-364B-8235-7C4E537AA579}" name="clubs in app" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{07E2AC0A-3AAB-F444-902C-A129018B5327}" name="clubs in afdeling" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{87F1F381-FA3E-8D40-851D-A4F7993752DE}" name="Fotobond" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{A9CF5635-EBAD-B040-BF71-3E77E09BBB43}" name="nonFotobond" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{5C084667-3F83-6F4E-8687-1A7FBBF558C2}" name="% Fotobond" dataDxfId="3" dataCellStyle="Percent"/>
+    <tableColumn id="7" xr3:uid="{24532655-7031-274B-854D-128E98E3B718}" name="Moment actief" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{A8142398-B094-F849-B96E-739B6E42C1DA}" name="Opmerking" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0EC1E894-FF62-D94F-86C9-0F118170FA74}" name="Table2" displayName="Table2" ref="B3:D17" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0EC1E894-FF62-D94F-86C9-0F118170FA74}" name="Table2" displayName="Table2" ref="B3:D17" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="B3:D17" xr:uid="{0EC1E894-FF62-D94F-86C9-0F118170FA74}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8B16138C-6720-474D-87C6-17E647EE5905}" name="beheerder"/>
@@ -1383,8 +1419,8 @@
   </sheetPr>
   <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="141" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="141" workbookViewId="0">
+      <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1424,7 +1460,7 @@
       <c r="D3" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="G3" s="46"/>
+      <c r="G3" s="42"/>
     </row>
     <row r="4" spans="1:7">
       <c r="B4" t="s">
@@ -1500,7 +1536,7 @@
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1511,7 +1547,7 @@
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1522,7 +1558,7 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1533,7 +1569,7 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1555,7 +1591,7 @@
         <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1566,12 +1602,12 @@
         <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:17">
       <c r="B18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C18">
         <f>SUM(C4:C17)</f>
@@ -1580,7 +1616,7 @@
     </row>
     <row r="19" spans="1:17">
       <c r="B19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C19">
         <f>SUM(C5:C8)-C8</f>
@@ -1591,21 +1627,21 @@
     <row r="21" spans="1:17" s="7" customFormat="1" ht="17" thickTop="1">
       <c r="A21"/>
       <c r="B21"/>
-      <c r="C21" s="44" t="s">
-        <v>86</v>
-      </c>
-      <c r="D21" s="42"/>
-      <c r="E21" s="41" t="s">
+      <c r="C21" s="50" t="s">
+        <v>85</v>
+      </c>
+      <c r="D21" s="48"/>
+      <c r="E21" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="F21" s="42"/>
-      <c r="G21" s="41" t="s">
+      <c r="F21" s="48"/>
+      <c r="G21" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="H21" s="43"/>
-      <c r="I21" s="43"/>
-      <c r="J21" s="43"/>
-      <c r="K21" s="42"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="49"/>
+      <c r="K21" s="48"/>
       <c r="L21" s="38" t="s">
         <v>46</v>
       </c>
@@ -1635,7 +1671,7 @@
         <v>54</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H22" s="16" t="s">
         <v>29</v>
@@ -1681,7 +1717,7 @@
       <c r="F23" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="G23" s="45" t="s">
+      <c r="G23" s="41" t="s">
         <v>19</v>
       </c>
       <c r="H23" s="3" t="s">
@@ -1709,7 +1745,7 @@
         <v>74</v>
       </c>
       <c r="B24" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="C24" s="24">
         <v>1</v>
@@ -1723,7 +1759,7 @@
       <c r="F24" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G24" s="47" t="s">
+      <c r="G24" s="43" t="s">
         <v>25</v>
       </c>
       <c r="H24" s="3" t="s">
@@ -1745,7 +1781,7 @@
         <v>18</v>
       </c>
       <c r="N24" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:17" ht="20" customHeight="1">
@@ -1767,7 +1803,7 @@
       <c r="F25" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="G25" s="45" t="s">
+      <c r="G25" s="41" t="s">
         <v>18</v>
       </c>
       <c r="H25" s="3" t="s">
@@ -1806,7 +1842,7 @@
       <c r="F26" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G26" s="45" t="s">
+      <c r="G26" s="41" t="s">
         <v>18</v>
       </c>
       <c r="H26" s="3" t="s">
@@ -1850,7 +1886,7 @@
       <c r="F27" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G27" s="45" t="s">
+      <c r="G27" s="41" t="s">
         <v>18</v>
       </c>
       <c r="H27" s="3" t="s">
@@ -1889,7 +1925,7 @@
       <c r="F28" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G28" s="45" t="s">
+      <c r="G28" s="41" t="s">
         <v>18</v>
       </c>
       <c r="H28" s="3" t="s">
@@ -1928,7 +1964,7 @@
       <c r="F29" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="G29" s="45" t="s">
+      <c r="G29" s="41" t="s">
         <v>18</v>
       </c>
       <c r="H29" s="3" t="s">
@@ -1967,7 +2003,7 @@
       <c r="F30" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G30" s="45" t="s">
+      <c r="G30" s="41" t="s">
         <v>25</v>
       </c>
       <c r="H30" s="3" t="s">
@@ -1994,44 +2030,44 @@
     </row>
     <row r="31" spans="1:17" ht="20" customHeight="1">
       <c r="A31" s="35" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B31" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="C31" s="48">
+      <c r="C31" s="44">
         <v>1</v>
       </c>
-      <c r="D31" s="49">
+      <c r="D31" s="45">
         <v>16</v>
       </c>
       <c r="E31" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F31" s="49" t="s">
-        <v>18</v>
-      </c>
-      <c r="G31" s="45" t="s">
+      <c r="F31" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="H31" s="47" t="s">
-        <v>19</v>
-      </c>
-      <c r="I31" s="47" t="s">
-        <v>19</v>
-      </c>
-      <c r="J31" s="47" t="s">
-        <v>19</v>
-      </c>
-      <c r="K31" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="L31" s="50" t="s">
-        <v>19</v>
-      </c>
-      <c r="M31" s="47"/>
+      <c r="H31" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="I31" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="J31" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="K31" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="L31" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="M31" s="43"/>
       <c r="N31" s="35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:17" ht="20" customHeight="1">
@@ -2053,7 +2089,7 @@
       <c r="F32" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G32" s="45" t="s">
+      <c r="G32" s="41" t="s">
         <v>18</v>
       </c>
       <c r="H32" s="3" t="s">
@@ -2075,7 +2111,7 @@
     </row>
     <row r="33" spans="1:14" ht="20" customHeight="1">
       <c r="A33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B33" t="s">
         <v>14</v>
@@ -2092,7 +2128,7 @@
       <c r="F33" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="G33" s="45" t="s">
+      <c r="G33" s="41" t="s">
         <v>18</v>
       </c>
       <c r="H33" s="3" t="s">
@@ -2116,7 +2152,7 @@
     </row>
     <row r="34" spans="1:14" ht="20" customHeight="1">
       <c r="A34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B34" t="s">
         <v>15</v>
@@ -2133,7 +2169,7 @@
       <c r="F34" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="G34" s="45" t="s">
+      <c r="G34" s="41" t="s">
         <v>25</v>
       </c>
       <c r="H34" s="3" t="s">
@@ -2155,10 +2191,10 @@
     </row>
     <row r="35" spans="1:14" ht="20" customHeight="1">
       <c r="A35" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B35" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C35" s="24">
         <v>1</v>
@@ -2172,7 +2208,7 @@
       <c r="F35" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G35" s="45" t="s">
+      <c r="G35" s="41" t="s">
         <v>25</v>
       </c>
       <c r="H35" s="3" t="s">
@@ -2192,7 +2228,7 @@
       </c>
       <c r="M35" s="3"/>
       <c r="N35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="20" customHeight="1">
@@ -2214,7 +2250,7 @@
       <c r="F36" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="G36" s="45" t="s">
+      <c r="G36" s="41" t="s">
         <v>18</v>
       </c>
       <c r="H36" s="3" t="s">
@@ -2255,7 +2291,7 @@
       <c r="F37" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G37" s="45" t="s">
+      <c r="G37" s="41" t="s">
         <v>18</v>
       </c>
       <c r="H37" s="3" t="s">
@@ -2314,7 +2350,7 @@
     </row>
     <row r="40" spans="1:14" ht="18" thickTop="1" thickBot="1">
       <c r="A40" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C40" s="40">
         <f>1 - C39/D39</f>
@@ -2402,7 +2438,7 @@
         <v>31</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G44" s="32" t="e">
         <f>Table5[[#This Row],[Fotobond]]/(Table5[[#This Row],[Fotobond]]+Table5[[#This Row],[nonFotobond]])</f>
@@ -2500,14 +2536,14 @@
     </row>
     <row r="49" spans="1:9" ht="18" thickTop="1" thickBot="1">
       <c r="A49" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C49" s="40">
         <f>1 - C48/D48</f>
         <v>0.2583333333333333</v>
       </c>
       <c r="I49" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="17" thickTop="1"/>

</xml_diff>

<commit_message>
Updated ClubsNL spreadsheet for fcVeghel
</commit_message>
<xml_diff>
--- a/JSON/ClubsNL.xlsx
+++ b/JSON/ClubsNL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petervandenhamer/Developer/Xcode projects/SwiftUI/Photo-Club-Hub/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D4D29F-0605-7D4A-AA86-ABDDC84BBADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC0C91F-7814-F541-89DC-6DD85B503E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="600" windowWidth="51200" windowHeight="26400" xr2:uid="{084E1DFC-5E29-0141-8377-174496560C67}"/>
   </bookViews>
@@ -1420,7 +1420,7 @@
   <dimension ref="A1:Q50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" zoomScale="141" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27"/>
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1747,11 +1747,11 @@
       <c r="B24" t="s">
         <v>95</v>
       </c>
-      <c r="C24" s="24">
-        <v>1</v>
+      <c r="C24" s="21">
+        <v>28</v>
       </c>
       <c r="D24" s="13">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E24" s="12" t="s">
         <v>18</v>
@@ -1760,7 +1760,7 @@
         <v>18</v>
       </c>
       <c r="G24" s="43" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>19</v>
@@ -2332,11 +2332,11 @@
       </c>
       <c r="C39" s="9">
         <f>SUM(C23:C37)</f>
-        <v>141</v>
+        <v>168</v>
       </c>
       <c r="D39" s="9">
         <f>SUM(D23:D37)</f>
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E39" s="14"/>
       <c r="F39" s="15"/>
@@ -2354,7 +2354,7 @@
       </c>
       <c r="C40" s="40">
         <f>1 - C39/D39</f>
-        <v>0.4173553719008265</v>
+        <v>0.28510638297872337</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="17" thickTop="1">
@@ -2554,7 +2554,7 @@
     <mergeCell ref="C21:D21"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G24" r:id="rId1" xr:uid="{6B877BCA-FAC0-CA45-A9F8-5DB8E2862E74}"/>
+    <hyperlink ref="G24" r:id="rId1" display="incompleet" xr:uid="{6B877BCA-FAC0-CA45-A9F8-5DB8E2862E74}"/>
     <hyperlink ref="G30" r:id="rId2" xr:uid="{EA518462-58C1-0D43-AFAB-D0D435BCFCF8}"/>
     <hyperlink ref="G31" r:id="rId3" xr:uid="{D509616D-ADA9-DE4E-85FF-FE0FAAE01599}"/>
     <hyperlink ref="G34" r:id="rId4" xr:uid="{C029A8E2-CAAD-E34C-A625-21082F80D214}"/>

</xml_diff>

<commit_message>
Added some minor comments.
</commit_message>
<xml_diff>
--- a/JSON/ClubsNL.xlsx
+++ b/JSON/ClubsNL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petervandenhamer/Developer/Xcode projects/SwiftUI/Photo-Club-Hub/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC0C91F-7814-F541-89DC-6DD85B503E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70D90CDF-C0F9-5A4F-9166-7D4F2E1BAD76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="600" windowWidth="51200" windowHeight="26400" xr2:uid="{084E1DFC-5E29-0141-8377-174496560C67}"/>
   </bookViews>
@@ -1420,7 +1420,7 @@
   <dimension ref="A1:Q50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" zoomScale="141" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1748,10 +1748,10 @@
         <v>95</v>
       </c>
       <c r="C24" s="21">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="D24" s="13">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="E24" s="12" t="s">
         <v>18</v>
@@ -2332,11 +2332,11 @@
       </c>
       <c r="C39" s="9">
         <f>SUM(C23:C37)</f>
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="D39" s="9">
         <f>SUM(D23:D37)</f>
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="E39" s="14"/>
       <c r="F39" s="15"/>
@@ -2354,7 +2354,7 @@
       </c>
       <c r="C40" s="40">
         <f>1 - C39/D39</f>
-        <v>0.28510638297872337</v>
+        <v>0.27685950413223137</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="17" thickTop="1">

</xml_diff>

<commit_message>
Update of ClubsNL spreadsheet
</commit_message>
<xml_diff>
--- a/JSON/ClubsNL.xlsx
+++ b/JSON/ClubsNL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petervandenhamer/Developer/Xcode projects/SwiftUI/Photo-Club-Hub/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70D90CDF-C0F9-5A4F-9166-7D4F2E1BAD76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A5B9652-910D-7A46-84D2-0598EF1301AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="600" windowWidth="51200" windowHeight="26400" xr2:uid="{084E1DFC-5E29-0141-8377-174496560C67}"/>
   </bookViews>
@@ -1420,7 +1420,7 @@
   <dimension ref="A1:Q50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" zoomScale="141" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1831,10 +1831,10 @@
         <v>8</v>
       </c>
       <c r="C26" s="21">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D26" s="13">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E26" s="12" t="s">
         <v>18</v>
@@ -2332,11 +2332,11 @@
       </c>
       <c r="C39" s="9">
         <f>SUM(C23:C37)</f>
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D39" s="9">
         <f>SUM(D23:D37)</f>
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="E39" s="14"/>
       <c r="F39" s="15"/>
@@ -2354,7 +2354,7 @@
       </c>
       <c r="C40" s="40">
         <f>1 - C39/D39</f>
-        <v>0.27685950413223137</v>
+        <v>0.27459016393442626</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="17" thickTop="1">

</xml_diff>

<commit_message>
Reduced size of color picker palette from 48 to 12 colors. The removed 36 colors were transparent versions of the first 12.
</commit_message>
<xml_diff>
--- a/JSON/ClubsNL.xlsx
+++ b/JSON/ClubsNL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petervandenhamer/Developer/Xcode projects/SwiftUI/Photo-Club-Hub/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD922DE-343A-A948-9D41-1944CEE33BD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F43AFF5-1521-1F48-864D-649D631AF577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="600" windowWidth="51200" windowHeight="26400" xr2:uid="{084E1DFC-5E29-0141-8377-174496560C67}"/>
   </bookViews>
@@ -403,7 +403,7 @@
     <t>Harry Michiels</t>
   </si>
   <si>
-    <t>besproken/goedgekeurd in ALV op 5-Feb-26</t>
+    <t>besproken/goedgekeurd op club ALV op 5-Feb-26</t>
   </si>
 </sst>
 </file>
@@ -1420,7 +1420,7 @@
   <dimension ref="A1:Q50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" zoomScale="141" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+      <selection activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1766,13 +1766,13 @@
         <v>28</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="J24" s="26" t="s">
         <v>19</v>
       </c>
       <c r="K24" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L24" s="3" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
ClubsNL speadsheet (very minor change)
</commit_message>
<xml_diff>
--- a/JSON/ClubsNL.xlsx
+++ b/JSON/ClubsNL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10222"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petervandenhamer/Developer/Xcode projects/SwiftUI/Photo-Club-Hub/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F43AFF5-1521-1F48-864D-649D631AF577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56737D37-1151-134A-B046-3B906C498E4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="51200" windowHeight="26400" xr2:uid="{084E1DFC-5E29-0141-8377-174496560C67}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="29400" windowHeight="16660" xr2:uid="{084E1DFC-5E29-0141-8377-174496560C67}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1419,8 +1419,8 @@
   </sheetPr>
   <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="141" workbookViewId="0">
-      <selection activeCell="Q27" sqref="Q27"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="141" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1768,8 +1768,8 @@
       <c r="I24" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="J24" s="26" t="s">
-        <v>19</v>
+      <c r="J24" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="K24" s="25" t="s">
         <v>18</v>

</xml_diff>